<commit_message>
Change names from MSE to mean distance. Fix mean distance plots.
</commit_message>
<xml_diff>
--- a/data/experiments/footage_experiments.xlsx
+++ b/data/experiments/footage_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\pitchmap\data\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99B3429-A0EF-47F6-9808-FCC16C483B97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFFEC30-845B-46CD-A277-5EC6005F7FFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="batch_iou_homographies" sheetId="1" r:id="rId1"/>
@@ -67,9 +67,6 @@
     <t>IoU</t>
   </si>
   <si>
-    <t>MSE</t>
-  </si>
-  <si>
     <t>Liczba klatek</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>Łącznie (średnia metryk, łączna liczba klatek)</t>
+  </si>
+  <si>
+    <t>Średni błąd [m]</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,17 +947,17 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -998,13 +998,13 @@
         <v>0.97793221476650805</v>
       </c>
       <c r="G3">
-        <v>553.5494089</v>
+        <v>5.1212542330011503</v>
       </c>
       <c r="H3">
-        <v>599.39196939999999</v>
+        <v>5.70055632427436</v>
       </c>
       <c r="I3">
-        <v>135.5933201</v>
+        <v>2.8685542400222799</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1027,13 +1027,13 @@
         <v>0.96829441743689704</v>
       </c>
       <c r="G4">
-        <v>255.33451070000001</v>
+        <v>3.64492172581136</v>
       </c>
       <c r="H4">
-        <v>1203.1000019999999</v>
+        <v>7.8288251408595002</v>
       </c>
       <c r="I4">
-        <v>126.7281705</v>
+        <v>2.8308090215864898</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1056,13 +1056,13 @@
         <v>0.96119333561921005</v>
       </c>
       <c r="G5">
-        <v>899.77653510000005</v>
+        <v>7.0710577745182297</v>
       </c>
       <c r="H5">
-        <v>1038.81014</v>
+        <v>7.57451590247853</v>
       </c>
       <c r="I5">
-        <v>215.65074379999999</v>
+        <v>3.4753383706745602</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1085,13 +1085,13 @@
         <v>0.96963368871696098</v>
       </c>
       <c r="G6">
-        <v>336.50506680000001</v>
+        <v>4.10133794441413</v>
       </c>
       <c r="H6">
-        <v>436.47888819999997</v>
+        <v>5.1066861988382399</v>
       </c>
       <c r="I6">
-        <v>129.9670764</v>
+        <v>2.7233334868241799</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1114,13 +1114,13 @@
         <v>0.93961924904661898</v>
       </c>
       <c r="G7">
-        <v>800.96255659999997</v>
+        <v>6.3848101617108197</v>
       </c>
       <c r="H7">
-        <v>575.83130819999997</v>
+        <v>5.1968136425635096</v>
       </c>
       <c r="I7">
-        <v>157.6799676</v>
+        <v>3.1215626569230701</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1143,13 +1143,13 @@
         <v>0.979354741843521</v>
       </c>
       <c r="G8">
-        <v>459.08156380000003</v>
+        <v>4.58888371465234</v>
       </c>
       <c r="H8">
-        <v>594.7542641</v>
+        <v>5.7132084943813304</v>
       </c>
       <c r="I8">
-        <v>344.26594019999999</v>
+        <v>4.6267269125742603</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1172,13 +1172,13 @@
         <v>0.99146940292952002</v>
       </c>
       <c r="G9">
-        <v>272.04130889999999</v>
+        <v>4.2963607144986398</v>
       </c>
       <c r="H9">
-        <v>197.1211218</v>
+        <v>3.6083834453795101</v>
       </c>
       <c r="I9">
-        <v>111.4824694</v>
+        <v>2.5241108252828299</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1201,13 +1201,13 @@
         <v>0.99184919910935199</v>
       </c>
       <c r="G10">
-        <v>114.45415180000001</v>
+        <v>2.41677326657488</v>
       </c>
       <c r="H10">
-        <v>169.46369240000001</v>
+        <v>3.3237553242971298</v>
       </c>
       <c r="I10">
-        <v>200.43397279999999</v>
+        <v>3.3458391518149702</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1230,13 +1230,13 @@
         <v>0.89167328870023399</v>
       </c>
       <c r="G11">
-        <v>1841.731086</v>
+        <v>8.0934972050308005</v>
       </c>
       <c r="H11">
-        <v>1371.2132790000001</v>
+        <v>6.7694905765076099</v>
       </c>
       <c r="I11">
-        <v>1821.41274</v>
+        <v>12.3995980610463</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1259,13 +1259,13 @@
         <v>0.91157540945818505</v>
       </c>
       <c r="G12">
-        <v>1594.0641479999999</v>
+        <v>8.1189668947355607</v>
       </c>
       <c r="H12">
-        <v>2642.0751249999998</v>
+        <v>11.2097337141926</v>
       </c>
       <c r="I12">
-        <v>2145.386524</v>
+        <v>9.5129165829411697</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1288,18 +1288,18 @@
         <v>0.923556499768726</v>
       </c>
       <c r="G13">
-        <v>2397.0283079999999</v>
+        <v>9.0785509484252493</v>
       </c>
       <c r="H13">
-        <v>3109.181372</v>
+        <v>10.472118526196899</v>
       </c>
       <c r="I13">
-        <v>2653.953794</v>
+        <v>10.0935328105118</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <f>SUM(C3:C13)</f>
@@ -1319,15 +1319,15 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>865.86624041818175</v>
+        <v>5.7196740530339234</v>
       </c>
       <c r="H14" s="1">
         <f>AVERAGE(H3:H13)</f>
-        <v>1085.2201056454544</v>
+        <v>6.5912806627244747</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>731.14133807272719</v>
+        <v>5.2293020109274462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>